<commit_message>
error handling on scrapper_Service
</commit_message>
<xml_diff>
--- a/public/uploads/attachment/file/18/PHOENIX_CONTACT_cesta_de_productos_exportación_2022-12-08.xlsx
+++ b/public/uploads/attachment/file/18/PHOENIX_CONTACT_cesta_de_productos_exportación_2022-12-08.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">3273112</t>
+    <t xml:space="preserve">3273114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6SL32105BE211UV0</t>
   </si>
 </sst>
 </file>
@@ -32,7 +35,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -54,6 +57,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,8 +109,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -126,16 +145,20 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="n">
-        <v>5</v>
+      <c r="B1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>